<commit_message>
Se modifica DataTable para ejecucion
</commit_message>
<xml_diff>
--- a/Default.xlsx
+++ b/Default.xlsx
@@ -1,166 +1,45 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fileVersion appName="SpreadsheetGear 8.2.5.102"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18075" windowHeight="9900" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18075" windowHeight="9900"/>
   </bookViews>
   <sheets>
     <sheet name="Global" sheetId="1" r:id="rId1"/>
     <sheet name="Action1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="40001"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="5">
-  <si>
-    <t>Gatos</t>
-  </si>
-  <si>
-    <t>Cortinas</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>p_palabra</t>
   </si>
   <si>
-    <t>Perros</t>
+    <t>Gallina</t>
   </si>
   <si>
-    <t>Celular</t>
+    <t>Caballo</t>
+  </si>
+  <si>
+    <t>Karting</t>
+  </si>
+  <si>
+    <t>Teclado</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="17">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri Light"/>
-      <scheme val="major"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -211,6 +90,8 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
@@ -502,42 +383,43 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1">
-      <c t="s">
+    <row r="1" spans="1:1" customFormat="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row>
-      <c s="2" t="s">
+    <row r="4" spans="1:1">
+      <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row>
-      <c s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row>
-      <c s="2" t="s">
+    <row r="5" spans="1:1">
+      <c r="A5" s="2" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row>
-      <c s="2" t="s">
-        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -546,19 +428,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1"/>
+    <row r="1" customFormat="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Se modifica DataTable previo a la ejecucion
</commit_message>
<xml_diff>
--- a/Default.xlsx
+++ b/Default.xlsx
@@ -20,16 +20,16 @@
     <t>p_palabra</t>
   </si>
   <si>
-    <t>Gallina</t>
+    <t>Gato</t>
   </si>
   <si>
-    <t>Caballo</t>
+    <t>Arquero</t>
   </si>
   <si>
-    <t>Karting</t>
+    <t>Ficha</t>
   </si>
   <si>
-    <t>Teclado</t>
+    <t>Poker</t>
   </si>
 </sst>
 </file>
@@ -387,7 +387,7 @@
   <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -414,12 +414,12 @@
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>